<commit_message>
Add Spring Boot project and start work on points request validation
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">Total hours:</t>
   </si>
@@ -40,13 +40,19 @@
     <t xml:space="preserve">Desc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Projektin käynnistys</t>
+    <t xml:space="preserve">Frontin käynnistys</t>
   </si>
   <si>
     <t xml:space="preserve">Frontti ohjelmointi</t>
   </si>
   <si>
     <t xml:space="preserve">Github ongelmia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bäkkärin käynnistys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bäkkäri ohjelmointi</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,10 +152,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,7 +295,7 @@
       </c>
       <c r="B1" s="1" t="n">
         <f aca="false">SUM(D:D)</f>
-        <v>0.520833333333333</v>
+        <v>0.628472222222222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,7 +388,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="4" t="n">
         <v>46034</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -399,12 +401,12 @@
         <f aca="false">C8-B8</f>
         <v>0.125</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="4" t="n">
         <v>46034</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -417,8 +419,44 @@
         <f aca="false">C9-B9</f>
         <v>0.0208333333333333</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0.65625</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <f aca="false">C10-B10</f>
+        <v>0.03125</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>46035</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.847222222222222</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="false">C11-B11</f>
+        <v>0.0763888888888889</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>